<commit_message>
[doc] update _weekly.txt and N2Team_WeeklySchedule_LJJ.xlsx
</commit_message>
<xml_diff>
--- a/doc/_meeting_weekly_doc/N2Team_WeeklySchedule_LJJ.xlsx
+++ b/doc/_meeting_weekly_doc/N2Team_WeeklySchedule_LJJ.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="27900" windowHeight="3600" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="27900" windowHeight="3600" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="2" sheetId="1" r:id="rId1"/>
     <sheet name="3" sheetId="4" r:id="rId2"/>
     <sheet name="4" sheetId="5" r:id="rId3"/>
     <sheet name="5" sheetId="6" r:id="rId4"/>
+    <sheet name="6" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="110">
   <si>
     <t xml:space="preserve">작성자 </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -412,6 +413,66 @@
   </si>
   <si>
     <t>조명연구 &amp; 테스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.28 ~ 12.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 총기부착, 조명연구, GUI 툴 마무리.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 등원 못함. 병원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI툴 버그 수정 &amp; 화면 크기에 따라 스케일 조정 하는 내용 구현.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캐릭터 총기부착 연구, 구현. 캐릭터 총기 발사 애니메이션 보간 연구, 구현. UI버튼 눌렀을때 PS에서 색깔처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI 버튼 눌렀을때 셰이더에서 색깔처리 구현. 엔진과 연동 테스트. 디버깅.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>집안일. 병원방문.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>없음.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>집안일. 병원방문.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>차주에 총기부착, 조명 구현 완료해야함.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>총기부착, 조명 구현, 그림자, OBBvsOBB충돌시 슬라이딩 벡터 계산 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캐릭터 조명 연구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캐릭터 조명 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그림자 연구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그림자 구현. OBB vs OBB 충돌시 슬라이딩 벡터 계산 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1119,6 +1180,126 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1131,125 +1312,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1259,27 +1341,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1608,292 +1669,292 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" thickBot="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" thickTop="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="24" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="32"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="50"/>
       <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="25"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" spans="1:8" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="48"/>
+      <c r="C3" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="41"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="46"/>
     </row>
     <row r="5" spans="1:8" ht="45" customHeight="1" thickTop="1">
-      <c r="A5" s="38">
+      <c r="A5" s="22">
         <v>42674</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A6" s="39"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="52"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A7" s="40"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="47"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A8" s="41">
+      <c r="A8" s="25">
         <v>42675</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A9" s="42"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="52"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A10" s="43"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="47"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A11" s="41">
+      <c r="A11" s="25">
         <v>42676</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="37"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
     </row>
     <row r="12" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A12" s="42"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="52"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A13" s="43"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="47"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A14" s="41">
+      <c r="A14" s="25">
         <v>42677</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A15" s="42"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="52"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A16" s="43"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="47"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="1:8" ht="18" thickTop="1">
-      <c r="A17" s="39">
+      <c r="A17" s="23">
         <v>42678</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="49"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="33"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="39"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="52"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A19" s="44"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="52"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" ht="50.25" customHeight="1">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="53" t="s">
+      <c r="B20" s="19"/>
+      <c r="C20" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="55"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="6">
@@ -1902,14 +1963,14 @@
       <c r="B21" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="13"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="53"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="6">
@@ -1918,14 +1979,14 @@
       <c r="B22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="13"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="53"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="6">
@@ -1934,14 +1995,14 @@
       <c r="B23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="13"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="53"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="6">
@@ -1950,14 +2011,14 @@
       <c r="B24" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="13"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="53"/>
     </row>
     <row r="25" spans="1:8" ht="17.25" thickBot="1">
       <c r="A25" s="8">
@@ -1966,26 +2027,33 @@
       <c r="B25" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="15"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="55"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A5:A7"/>
@@ -2002,19 +2070,12 @@
     <mergeCell ref="C16:H16"/>
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="C6:H6"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C18:H18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2042,85 +2103,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" thickBot="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" thickTop="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="24" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="32"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="50"/>
       <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="25"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" spans="1:8" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="48"/>
+      <c r="C3" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="41"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="38"/>
+      <c r="C4" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="46"/>
     </row>
     <row r="5" spans="1:8" ht="52.5" customHeight="1" thickTop="1">
-      <c r="A5" s="38">
+      <c r="A5" s="22">
         <v>42674</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="65"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="58"/>
     </row>
     <row r="6" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A6" s="39"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="59" t="s">
         <v>55</v>
       </c>
       <c r="D6" s="60"/>
@@ -2130,41 +2191,41 @@
       <c r="H6" s="61"/>
     </row>
     <row r="7" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A7" s="40"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="47"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A8" s="41">
+      <c r="A8" s="25">
         <v>42675</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="58"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="65"/>
     </row>
     <row r="9" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A9" s="42"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="62" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="60"/>
@@ -2174,41 +2235,41 @@
       <c r="H9" s="61"/>
     </row>
     <row r="10" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A10" s="43"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="47"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A11" s="41">
+      <c r="A11" s="25">
         <v>42676</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="58"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="65"/>
     </row>
     <row r="12" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A12" s="42"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="62" t="s">
         <v>49</v>
       </c>
       <c r="D12" s="60"/>
@@ -2218,41 +2279,41 @@
       <c r="H12" s="61"/>
     </row>
     <row r="13" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A13" s="43"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="47"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A14" s="41">
+      <c r="A14" s="25">
         <v>42677</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="56" t="s">
+      <c r="C14" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="58"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="65"/>
     </row>
     <row r="15" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A15" s="42"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="59" t="s">
+      <c r="C15" s="62" t="s">
         <v>46</v>
       </c>
       <c r="D15" s="60"/>
@@ -2262,41 +2323,41 @@
       <c r="H15" s="61"/>
     </row>
     <row r="16" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A16" s="43"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="47"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="1:8" ht="18" customHeight="1" thickTop="1">
-      <c r="A17" s="39">
+      <c r="A17" s="23">
         <v>42678</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="58"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="65"/>
     </row>
     <row r="18" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A18" s="39"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="62" t="s">
         <v>43</v>
       </c>
       <c r="D18" s="60"/>
@@ -2306,32 +2367,32 @@
       <c r="H18" s="61"/>
     </row>
     <row r="19" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A19" s="44"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="50" t="s">
+      <c r="C19" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="52"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" ht="32.25" customHeight="1">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="53" t="s">
+      <c r="B20" s="19"/>
+      <c r="C20" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="55"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="6">
@@ -2340,14 +2401,14 @@
       <c r="B21" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="13"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="53"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="6">
@@ -2356,14 +2417,14 @@
       <c r="B22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="13"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="53"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="6">
@@ -2372,14 +2433,14 @@
       <c r="B23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="13"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="53"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="6">
@@ -2388,14 +2449,14 @@
       <c r="B24" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="13"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="53"/>
     </row>
     <row r="25" spans="1:8" ht="17.25" thickBot="1">
       <c r="A25" s="8">
@@ -2404,33 +2465,26 @@
       <c r="B25" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="15"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="55"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A5:A7"/>
@@ -2447,12 +2501,19 @@
     <mergeCell ref="C10:H10"/>
     <mergeCell ref="C11:H11"/>
     <mergeCell ref="C13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2480,85 +2541,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" thickBot="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" thickTop="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="24" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="32"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="50"/>
       <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="25"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" spans="1:8" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="48"/>
+      <c r="C3" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="41"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="38"/>
+      <c r="C4" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="46"/>
     </row>
     <row r="5" spans="1:8" ht="52.5" customHeight="1" thickTop="1">
-      <c r="A5" s="38">
+      <c r="A5" s="22">
         <v>42688</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="65"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="58"/>
     </row>
     <row r="6" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A6" s="39"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="59" t="s">
         <v>75</v>
       </c>
       <c r="D6" s="60"/>
@@ -2568,41 +2629,41 @@
       <c r="H6" s="61"/>
     </row>
     <row r="7" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A7" s="40"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="47"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A8" s="41">
+      <c r="A8" s="25">
         <v>42689</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="58"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="65"/>
     </row>
     <row r="9" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A9" s="42"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="62" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="60"/>
@@ -2612,41 +2673,41 @@
       <c r="H9" s="61"/>
     </row>
     <row r="10" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A10" s="43"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="47"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A11" s="41">
+      <c r="A11" s="25">
         <v>42690</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="58"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="65"/>
     </row>
     <row r="12" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A12" s="42"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="62" t="s">
         <v>70</v>
       </c>
       <c r="D12" s="60"/>
@@ -2656,41 +2717,41 @@
       <c r="H12" s="61"/>
     </row>
     <row r="13" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A13" s="43"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="47"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A14" s="41">
+      <c r="A14" s="25">
         <v>42691</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="56" t="s">
+      <c r="C14" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="58"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="65"/>
     </row>
     <row r="15" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A15" s="42"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="59" t="s">
+      <c r="C15" s="62" t="s">
         <v>67</v>
       </c>
       <c r="D15" s="60"/>
@@ -2700,41 +2761,41 @@
       <c r="H15" s="61"/>
     </row>
     <row r="16" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A16" s="43"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="47"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="1:8" ht="18" customHeight="1" thickTop="1">
-      <c r="A17" s="39">
+      <c r="A17" s="23">
         <v>42692</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="58"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="65"/>
     </row>
     <row r="18" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A18" s="39"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="62" t="s">
         <v>52</v>
       </c>
       <c r="D18" s="60"/>
@@ -2744,30 +2805,30 @@
       <c r="H18" s="61"/>
     </row>
     <row r="19" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A19" s="44"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="52"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" ht="32.25" customHeight="1">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="53" t="s">
+      <c r="B20" s="19"/>
+      <c r="C20" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="55"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="6">
@@ -2776,14 +2837,14 @@
       <c r="B21" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="13"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="53"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="6">
@@ -2792,14 +2853,14 @@
       <c r="B22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="13"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="53"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="6">
@@ -2808,14 +2869,14 @@
       <c r="B23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="13"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="53"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="6">
@@ -2824,14 +2885,14 @@
       <c r="B24" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="13"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="53"/>
     </row>
     <row r="25" spans="1:8" ht="17.25" thickBot="1">
       <c r="A25" s="8">
@@ -2840,20 +2901,39 @@
       <c r="B25" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="15"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="55"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C16:H16"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A5:A7"/>
@@ -2870,25 +2950,6 @@
     <mergeCell ref="C15:H15"/>
     <mergeCell ref="C20:H20"/>
     <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C25:H25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2903,8 +2964,8 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2916,85 +2977,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" thickBot="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" thickTop="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="24" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="32"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="50"/>
       <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="25"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" spans="1:8" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="48"/>
+      <c r="C3" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="41"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="38"/>
+      <c r="C4" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="46"/>
     </row>
     <row r="5" spans="1:8" ht="52.5" customHeight="1" thickTop="1">
-      <c r="A5" s="38">
+      <c r="A5" s="22">
         <v>42695</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="65"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="58"/>
     </row>
     <row r="6" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A6" s="39"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="62"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="60"/>
       <c r="E6" s="60"/>
       <c r="F6" s="60"/>
@@ -3002,39 +3063,39 @@
       <c r="H6" s="61"/>
     </row>
     <row r="7" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A7" s="40"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="47"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A8" s="41">
+      <c r="A8" s="25">
         <v>42696</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="58"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="65"/>
     </row>
     <row r="9" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A9" s="42"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="62" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="60"/>
@@ -3044,41 +3105,41 @@
       <c r="H9" s="61"/>
     </row>
     <row r="10" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A10" s="43"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="47"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A11" s="41">
+      <c r="A11" s="25">
         <v>42697</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="58"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="65"/>
     </row>
     <row r="12" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A12" s="42"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="62" t="s">
         <v>52</v>
       </c>
       <c r="D12" s="60"/>
@@ -3088,41 +3149,41 @@
       <c r="H12" s="61"/>
     </row>
     <row r="13" spans="1:8" ht="33" customHeight="1" thickBot="1">
-      <c r="A13" s="43"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="47"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:8" ht="54" customHeight="1" thickTop="1">
-      <c r="A14" s="41">
+      <c r="A14" s="25">
         <v>42698</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="56" t="s">
+      <c r="C14" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="58"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="65"/>
     </row>
     <row r="15" spans="1:8" ht="66.75" customHeight="1">
-      <c r="A15" s="42"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="59" t="s">
+      <c r="C15" s="62" t="s">
         <v>86</v>
       </c>
       <c r="D15" s="60"/>
@@ -3132,41 +3193,41 @@
       <c r="H15" s="61"/>
     </row>
     <row r="16" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A16" s="43"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="47"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="1:8" ht="18" customHeight="1" thickTop="1">
-      <c r="A17" s="39">
+      <c r="A17" s="23">
         <v>42699</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="58"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="65"/>
     </row>
     <row r="18" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A18" s="39"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="62" t="s">
         <v>52</v>
       </c>
       <c r="D18" s="60"/>
@@ -3176,32 +3237,32 @@
       <c r="H18" s="61"/>
     </row>
     <row r="19" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A19" s="44"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="50" t="s">
+      <c r="C19" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="52"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" ht="32.25" customHeight="1">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="53" t="s">
+      <c r="B20" s="19"/>
+      <c r="C20" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="55"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="6">
@@ -3288,18 +3349,21 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="C8:H8"/>
     <mergeCell ref="C9:H9"/>
@@ -3308,6 +3372,424 @@
     <mergeCell ref="C11:H11"/>
     <mergeCell ref="C12:H12"/>
     <mergeCell ref="C13:H13"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="82" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="12.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="9" style="4"/>
+    <col min="8" max="8" width="31.25" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="39" thickBot="1">
+      <c r="A1" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
+    </row>
+    <row r="2" spans="1:8" ht="17.25" thickTop="1">
+      <c r="A2" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="51"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="43"/>
+    </row>
+    <row r="3" spans="1:8" ht="56.25" customHeight="1" thickBot="1">
+      <c r="A3" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="48"/>
+      <c r="C3" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="41"/>
+    </row>
+    <row r="4" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A4" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="46"/>
+    </row>
+    <row r="5" spans="1:8" ht="52.5" customHeight="1" thickTop="1">
+      <c r="A5" s="22">
+        <v>42702</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="58"/>
+    </row>
+    <row r="6" spans="1:8" ht="37.5" customHeight="1">
+      <c r="A6" s="23"/>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="61"/>
+    </row>
+    <row r="7" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A7" s="24"/>
+      <c r="B7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
+    </row>
+    <row r="8" spans="1:8" ht="54" customHeight="1" thickTop="1">
+      <c r="A8" s="25">
+        <v>42703</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="58"/>
+    </row>
+    <row r="9" spans="1:8" ht="66.75" customHeight="1">
+      <c r="A9" s="26"/>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="61"/>
+    </row>
+    <row r="10" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A10" s="27"/>
+      <c r="B10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
+    </row>
+    <row r="11" spans="1:8" ht="54" customHeight="1" thickTop="1">
+      <c r="A11" s="25">
+        <v>42704</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="65"/>
+    </row>
+    <row r="12" spans="1:8" ht="66.75" customHeight="1">
+      <c r="A12" s="26"/>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="61"/>
+    </row>
+    <row r="13" spans="1:8" ht="33" customHeight="1" thickBot="1">
+      <c r="A13" s="27"/>
+      <c r="B13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
+    </row>
+    <row r="14" spans="1:8" ht="54" customHeight="1" thickTop="1">
+      <c r="A14" s="25">
+        <v>42705</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="65"/>
+    </row>
+    <row r="15" spans="1:8" ht="66.75" customHeight="1">
+      <c r="A15" s="26"/>
+      <c r="B15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="62" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="61"/>
+    </row>
+    <row r="16" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A16" s="27"/>
+      <c r="B16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
+    </row>
+    <row r="17" spans="1:8" ht="18" customHeight="1" thickTop="1">
+      <c r="A17" s="23">
+        <v>42706</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="65"/>
+    </row>
+    <row r="18" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A18" s="23"/>
+      <c r="B18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="61"/>
+    </row>
+    <row r="19" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A19" s="28"/>
+      <c r="B19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="1:8" ht="32.25" customHeight="1">
+      <c r="A20" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="19"/>
+      <c r="C20" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="6">
+        <v>42709</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="68" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="70"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="6">
+        <v>42710</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="68" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="70"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="6">
+        <v>42711</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="69" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="70"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="6">
+        <v>42712</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="69" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="70"/>
+    </row>
+    <row r="25" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A25" s="8">
+        <v>42713</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="66" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="67"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="C14:H14"/>
     <mergeCell ref="C15:H15"/>
@@ -3316,13 +3798,26 @@
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="C18:H18"/>
     <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>